<commit_message>
Probando de nuevo GIT como controlador de version
</commit_message>
<xml_diff>
--- a/SIAE/SNW/Reportes/Anexo2InventarioPTP.xlsx
+++ b/SIAE/SNW/Reportes/Anexo2InventarioPTP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvin Salinas\Desktop\Proyectos\ProyectoSIAE\SIAE\SNW\Reportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{18F73123-0514-48A7-B642-3379D71B6B50}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3387D8-5FCC-400F-921F-06985C862359}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,22 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'11 Serie Logística'!$A$1:$K$132</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Nombre Tecnico: ________________</t>
   </si>
@@ -70,9 +75,6 @@
   </si>
   <si>
     <t>Version 2</t>
-  </si>
-  <si>
-    <t>SI HAY CMM4 PEDIR CMM4 (Cambium),UGPS (Cambium) Y Conversor (Cambium) CASO CONTRARIO NO PEDIR Y LA REGLA PALICA PARA EL NODO B TAMBIEN</t>
   </si>
 </sst>
 </file>
@@ -149,7 +151,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,12 +167,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -426,9 +422,8 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,8 +460,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:M247"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A32" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75:XFD75"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A101" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:XFD97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -890,33 +884,33 @@
       <c r="M5" s="22"/>
     </row>
     <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="38"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="22"/>
     </row>
     <row r="7" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="41"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="40"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="22"/>
@@ -936,29 +930,29 @@
       <c r="M8" s="22"/>
     </row>
     <row r="9" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="32"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="2:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
@@ -993,13 +987,13 @@
       <c r="J15" s="12"/>
     </row>
     <row r="16" spans="2:13" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="43"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
       <c r="I16" s="1"/>
       <c r="J16" s="12"/>
     </row>
@@ -1257,18 +1251,16 @@
       <c r="I37" s="1"/>
       <c r="J37" s="12"/>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B38" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
+    <row r="38" spans="2:11" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="41"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="12"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="13"/>
@@ -1351,7 +1343,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:11" ht="166.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="13"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1431,7 +1423,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:11" ht="163.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="13"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -1464,7 +1456,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="12"/>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="11"/>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -1791,7 +1783,7 @@
       <c r="I83" s="1"/>
       <c r="J83" s="12"/>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:11" ht="169.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="13"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -1813,7 +1805,7 @@
       <c r="I85" s="1"/>
       <c r="J85" s="12"/>
     </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="11"/>
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
@@ -1872,7 +1864,7 @@
       <c r="I90" s="1"/>
       <c r="J90" s="12"/>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:11" ht="171.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="13"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -1941,7 +1933,7 @@
       <c r="I96" s="15"/>
       <c r="J96" s="14"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="13"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>

</xml_diff>